<commit_message>
Fix community name in excel data and update test exp value.
</commit_message>
<xml_diff>
--- a/tests/data/55+_Communities_v1.xlsx
+++ b/tests/data/55+_Communities_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/068c25a9d985af2b/Documents/Excel/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{0406E5C6-41FE-1A40-B1BC-525958FA3BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04A451AF-2331-42E4-BE7B-4F560F445067}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{0406E5C6-41FE-1A40-B1BC-525958FA3BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87255C30-8EB0-43F0-B16C-812F09F8CBAC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D8CA8855-D542-4F45-99A6-8DCF549F53DB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="127">
   <si>
     <t>Community Name</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Arizona Traditions</t>
-  </si>
-  <si>
-    <t>Glendale</t>
   </si>
   <si>
     <t>South Phoenix</t>
@@ -374,9 +371,6 @@
     <t>https://www.oursuncityfestival.net/</t>
   </si>
   <si>
-    <t>https://www.verrado.com/find-a-home/?neighborhood-victory&amp;utm_campaign=Low+Funnel+-+Search+-+Victory+Branded&amp;utm_term=victory%20at%20verrado&amp;utm_medium=ppc&amp;utm_source=adwords&amp;hsa_kw=victory%20at%20verrado&amp;hsa_mt=e&amp;hsa_grp=101515751279&amp;hsa_tgt=aud-1930006008419:kwd-347033056012&amp;hsa_net=adwords&amp;hsa_cam=10256924853&amp;hsa_ver=3&amp;hsa_acc=4564233426&amp;hsa_src=g&amp;hsa_ad=649719669784&amp;gad=1&amp;gclid=Cj0KCQjw1_SkBhDwARIsANbGpFtifZBiHk26qxEfeVXdRyp4HW-CWtIKp9YD5GI2ziSMPKEWwtaa-YEaAqETEALw_wcB</t>
-  </si>
-  <si>
     <t>https://www.sundanceadulthoa.org/</t>
   </si>
   <si>
@@ -416,16 +410,16 @@
     <t>https://www.dreamlandvilla.org/</t>
   </si>
   <si>
-    <t>Trilogy at Encanterra</t>
-  </si>
-  <si>
-    <t>https://www.sheahomes.com/new-homes/arizona/phoenix-area/queen-creek/encanterra-a-trilogy-resort-community/?utm_source=google&amp;utm_medium=CPC&amp;utm_campaign=SHALC_Arizona-(national)_(s)_P-Brand&amp;gclid=Cj0KCQjw1_SkBhDwARIsANbGpFvzmxstY6WOlRSdA9vc7OWOpnKdhKi82hLTC8dUGRw3e8q2-45Hd2oaAmaXEALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
     <t>https://www.johnsonranch.com/home/</t>
   </si>
   <si>
     <t>https://goldcanyon.net/gold-canyon-arizona-real-estate/subdivisions-and-communities/mountain-brook-village/</t>
+  </si>
+  <si>
+    <t>https://www.verrado.com/victory-at-verrado/</t>
+  </si>
+  <si>
+    <t>https://www.sheahomes.com/new-homes/arizona/phoenix-area/queen-creek/encanterra-a-trilogy-resort-community/</t>
   </si>
 </sst>
 </file>
@@ -539,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -622,10 +616,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,6 +644,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -952,10 +953,10 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -966,7 +967,7 @@
     <col min="7" max="8" width="20.796875" customWidth="1"/>
     <col min="9" max="9" width="14.796875" customWidth="1"/>
     <col min="10" max="10" width="15.19921875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="28.19921875" customWidth="1"/>
+    <col min="11" max="11" width="28.19921875" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -974,34 +975,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1036,7 +1037,7 @@
         <v>4000</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1044,7 +1045,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>4</v>
@@ -1071,7 +1072,7 @@
         <v>4200</v>
       </c>
       <c r="K3" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1079,7 +1080,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>4</v>
@@ -1106,15 +1107,15 @@
         <v>5000</v>
       </c>
       <c r="K4" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>4</v>
@@ -1141,15 +1142,15 @@
         <v>3750</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>4</v>
@@ -1176,15 +1177,15 @@
         <v>2000</v>
       </c>
       <c r="K6" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>4</v>
@@ -1211,15 +1212,15 @@
         <v>0</v>
       </c>
       <c r="K7" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>4</v>
@@ -1246,7 +1247,7 @@
         <v>1500</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1278,10 +1279,10 @@
         <v>2017</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
@@ -1313,10 +1314,10 @@
         <v>2019</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K10" s="32" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1351,7 +1352,7 @@
         <v>1700</v>
       </c>
       <c r="K11" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1362,7 +1363,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="12">
         <v>552000</v>
@@ -1386,7 +1387,7 @@
         <v>2728</v>
       </c>
       <c r="K12" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1421,7 +1422,7 @@
         <v>3680</v>
       </c>
       <c r="K13" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1456,7 +1457,7 @@
         <v>3360</v>
       </c>
       <c r="K14" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1464,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>4</v>
@@ -1491,18 +1492,18 @@
         <v>2100</v>
       </c>
       <c r="K15" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="12">
         <v>367000</v>
@@ -1526,18 +1527,18 @@
         <v>1050</v>
       </c>
       <c r="K16" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>21</v>
-      </c>
       <c r="C17" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="12">
         <v>476000</v>
@@ -1561,18 +1562,18 @@
         <v>5024</v>
       </c>
       <c r="K17" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>23</v>
-      </c>
       <c r="C18" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="12">
         <v>340000</v>
@@ -1596,18 +1597,18 @@
         <v>2800</v>
       </c>
       <c r="K18" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="12">
         <v>466000</v>
@@ -1631,18 +1632,18 @@
         <v>0</v>
       </c>
       <c r="K19" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>26</v>
-      </c>
       <c r="C20" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="12">
         <v>508000</v>
@@ -1666,18 +1667,18 @@
         <v>3275</v>
       </c>
       <c r="K20" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>28</v>
-      </c>
       <c r="C21" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="12">
         <v>555000</v>
@@ -1701,18 +1702,18 @@
         <v>612</v>
       </c>
       <c r="K21" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="12">
         <v>528000</v>
@@ -1736,18 +1737,18 @@
         <v>1197</v>
       </c>
       <c r="K22" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="12">
         <v>383000</v>
@@ -1771,18 +1772,18 @@
         <v>2000</v>
       </c>
       <c r="K23" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" s="12">
         <v>348000</v>
@@ -1806,18 +1807,18 @@
         <v>2025</v>
       </c>
       <c r="K24" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="12">
         <v>396000</v>
@@ -1841,18 +1842,18 @@
         <v>2000</v>
       </c>
       <c r="K25" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" s="12">
         <v>293000</v>
@@ -1875,19 +1876,19 @@
       <c r="J26" s="26">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
-        <v>124</v>
+      <c r="K26" s="33" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="12">
         <v>730000</v>
@@ -1916,13 +1917,13 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" s="26">
         <v>405000</v>
@@ -1945,19 +1946,19 @@
       <c r="J28" s="26">
         <v>1050</v>
       </c>
-      <c r="K28" t="s">
-        <v>127</v>
+      <c r="K28" s="33" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" s="26">
         <v>450000</v>
@@ -1980,8 +1981,8 @@
       <c r="J29" s="26">
         <v>1050</v>
       </c>
-      <c r="K29" s="32" t="s">
-        <v>128</v>
+      <c r="K29" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2080,58 +2081,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="N1" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -2145,49 +2146,49 @@
         <v>8</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="14">
         <v>130</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="14">
         <v>8</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S2" s="30">
         <v>4</v>
@@ -2204,49 +2205,49 @@
         <v>7</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="14">
         <v>100</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" s="14">
         <v>4</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S3" s="30">
         <v>5</v>
@@ -2263,49 +2264,49 @@
         <v>4</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="14">
         <v>45</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="14">
         <v>2</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S4" s="30">
         <v>5</v>
@@ -2313,7 +2314,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="21">
         <v>6600</v>
@@ -2322,49 +2323,49 @@
         <v>1</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="22">
         <v>10</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="22">
         <v>1</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N5" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S5" s="30">
         <v>3</v>
@@ -2372,58 +2373,58 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="22">
         <v>1</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="22">
         <v>0</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q6" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S6" s="30">
         <v>5</v>
@@ -2431,58 +2432,58 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="22">
         <v>0</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="22">
         <v>1</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P7" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S7" s="30">
         <v>1</v>
@@ -2490,58 +2491,58 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="14">
         <v>1</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" s="14">
         <v>1</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S8" s="30">
         <v>1</v>
@@ -2552,55 +2553,55 @@
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="14">
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="14">
         <v>25</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I9" s="14">
         <v>1</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S9" s="30">
         <v>3</v>
@@ -2617,49 +2618,49 @@
         <v>2</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I10" s="14">
         <v>3</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S10" s="30">
         <v>4</v>
@@ -2676,49 +2677,49 @@
         <v>1</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" s="14">
         <v>1</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S11" s="30">
         <v>3</v>
@@ -2735,49 +2736,49 @@
         <v>3</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I12" s="14">
         <v>2</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S12" s="30">
         <v>5</v>
@@ -2788,55 +2789,55 @@
         <v>13</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="14">
         <v>1</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I13" s="14">
         <v>1</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S13" s="30">
         <v>3</v>
@@ -2853,49 +2854,49 @@
         <v>1</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="14">
         <v>1</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q14" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R14" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S14" s="30">
         <v>3</v>
@@ -2912,49 +2913,49 @@
         <v>1</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="H15" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" s="14">
         <v>2</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P15" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q15" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R15" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S15" s="30">
         <v>2</v>
@@ -2962,7 +2963,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="13">
         <v>2000</v>
@@ -2971,49 +2972,49 @@
         <v>1</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I16" s="14">
         <v>1</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S16" s="30">
         <v>1</v>
@@ -3021,7 +3022,7 @@
     </row>
     <row r="17" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="13">
         <v>1100</v>
@@ -3030,49 +3031,49 @@
         <v>5</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I17" s="14">
         <v>3</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P17" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q17" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R17" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S17" s="30">
         <v>4</v>
@@ -3080,7 +3081,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="13">
         <v>2600</v>
@@ -3089,49 +3090,49 @@
         <v>1</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="14">
         <v>50</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="14">
         <v>1</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S18" s="30">
         <v>3</v>
@@ -3139,7 +3140,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="13">
         <v>2500</v>
@@ -3148,49 +3149,49 @@
         <v>1</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I19" s="14">
         <v>1</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P19" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q19" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R19" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S19" s="30">
         <v>3</v>
@@ -3198,58 +3199,58 @@
     </row>
     <row r="20" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="14">
         <v>1</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I20" s="14">
         <v>1</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S20" s="30">
         <v>4</v>
@@ -3257,58 +3258,58 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="14">
         <v>0</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="14">
         <v>30</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="14">
         <v>1</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N21" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q21" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R21" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S21" s="30">
         <v>4</v>
@@ -3316,7 +3317,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="13">
         <v>2450</v>
@@ -3325,49 +3326,49 @@
         <v>1</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I22" s="14">
         <v>2</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q22" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S22" s="30">
         <v>3</v>
@@ -3375,7 +3376,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="13">
         <v>2000</v>
@@ -3384,49 +3385,49 @@
         <v>1</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I23" s="14">
         <v>1</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N23" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S23" s="30">
         <v>2</v>
@@ -3434,7 +3435,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="13">
         <v>2425</v>
@@ -3443,49 +3444,49 @@
         <v>1</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24" s="14">
         <v>1</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q24" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S24" s="30">
         <v>3</v>
@@ -3493,7 +3494,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="13">
         <v>2568</v>
@@ -3502,49 +3503,49 @@
         <v>2</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" s="14">
         <v>1</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q25" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S25" s="30">
         <v>3</v>
@@ -3552,58 +3553,58 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="14">
         <v>0</v>
       </c>
       <c r="D26" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="F26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I26" s="14">
         <v>1</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P26" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q26" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S26" s="30">
         <v>3</v>
@@ -3611,7 +3612,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="21">
         <v>5520</v>
@@ -3620,49 +3621,49 @@
         <v>1</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I27" s="22">
         <v>2</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K27" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O27" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q27" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S27" s="30">
         <v>4</v>
@@ -3670,7 +3671,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="21">
         <v>4500</v>
@@ -3679,49 +3680,49 @@
         <v>1</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="22">
         <v>25</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I28" s="22">
         <v>1</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K28" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L28" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O28" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P28" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q28" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R28" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S28" s="30">
         <v>5</v>
@@ -3729,58 +3730,58 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="22">
         <v>1</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I29" s="22">
         <v>1</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K29" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L29" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M29" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q29" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R29" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S29" s="30">
         <v>2</v>
@@ -3806,7 +3807,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create the /update_data API endpoint (#13)
* Add new api and sfn resources to the template.

* Revise diagram to reflect latest architecture.

* Create Lambda to run the update data workflow.

* Create validate_community_data Lambda and tests.

* Create update_community_data Lambda to upload data to S3.

* Add custom exception when worksheets are not found.

* Increase poll frequency to improve performance for /rank endpoint.

* Fix community name in excel data and update test expected value.

* Factor out excel module.
</commit_message>
<xml_diff>
--- a/tests/data/55+_Communities_v1.xlsx
+++ b/tests/data/55+_Communities_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/068c25a9d985af2b/Documents/Excel/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{0406E5C6-41FE-1A40-B1BC-525958FA3BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04A451AF-2331-42E4-BE7B-4F560F445067}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{0406E5C6-41FE-1A40-B1BC-525958FA3BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87255C30-8EB0-43F0-B16C-812F09F8CBAC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D8CA8855-D542-4F45-99A6-8DCF549F53DB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="127">
   <si>
     <t>Community Name</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Arizona Traditions</t>
-  </si>
-  <si>
-    <t>Glendale</t>
   </si>
   <si>
     <t>South Phoenix</t>
@@ -374,9 +371,6 @@
     <t>https://www.oursuncityfestival.net/</t>
   </si>
   <si>
-    <t>https://www.verrado.com/find-a-home/?neighborhood-victory&amp;utm_campaign=Low+Funnel+-+Search+-+Victory+Branded&amp;utm_term=victory%20at%20verrado&amp;utm_medium=ppc&amp;utm_source=adwords&amp;hsa_kw=victory%20at%20verrado&amp;hsa_mt=e&amp;hsa_grp=101515751279&amp;hsa_tgt=aud-1930006008419:kwd-347033056012&amp;hsa_net=adwords&amp;hsa_cam=10256924853&amp;hsa_ver=3&amp;hsa_acc=4564233426&amp;hsa_src=g&amp;hsa_ad=649719669784&amp;gad=1&amp;gclid=Cj0KCQjw1_SkBhDwARIsANbGpFtifZBiHk26qxEfeVXdRyp4HW-CWtIKp9YD5GI2ziSMPKEWwtaa-YEaAqETEALw_wcB</t>
-  </si>
-  <si>
     <t>https://www.sundanceadulthoa.org/</t>
   </si>
   <si>
@@ -416,16 +410,16 @@
     <t>https://www.dreamlandvilla.org/</t>
   </si>
   <si>
-    <t>Trilogy at Encanterra</t>
-  </si>
-  <si>
-    <t>https://www.sheahomes.com/new-homes/arizona/phoenix-area/queen-creek/encanterra-a-trilogy-resort-community/?utm_source=google&amp;utm_medium=CPC&amp;utm_campaign=SHALC_Arizona-(national)_(s)_P-Brand&amp;gclid=Cj0KCQjw1_SkBhDwARIsANbGpFvzmxstY6WOlRSdA9vc7OWOpnKdhKi82hLTC8dUGRw3e8q2-45Hd2oaAmaXEALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
     <t>https://www.johnsonranch.com/home/</t>
   </si>
   <si>
     <t>https://goldcanyon.net/gold-canyon-arizona-real-estate/subdivisions-and-communities/mountain-brook-village/</t>
+  </si>
+  <si>
+    <t>https://www.verrado.com/victory-at-verrado/</t>
+  </si>
+  <si>
+    <t>https://www.sheahomes.com/new-homes/arizona/phoenix-area/queen-creek/encanterra-a-trilogy-resort-community/</t>
   </si>
 </sst>
 </file>
@@ -539,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -622,10 +616,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,6 +644,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -952,10 +953,10 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -966,7 +967,7 @@
     <col min="7" max="8" width="20.796875" customWidth="1"/>
     <col min="9" max="9" width="14.796875" customWidth="1"/>
     <col min="10" max="10" width="15.19921875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="28.19921875" customWidth="1"/>
+    <col min="11" max="11" width="28.19921875" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -974,34 +975,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1036,7 +1037,7 @@
         <v>4000</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1044,7 +1045,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>4</v>
@@ -1071,7 +1072,7 @@
         <v>4200</v>
       </c>
       <c r="K3" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1079,7 +1080,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>4</v>
@@ -1106,15 +1107,15 @@
         <v>5000</v>
       </c>
       <c r="K4" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>4</v>
@@ -1141,15 +1142,15 @@
         <v>3750</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>4</v>
@@ -1176,15 +1177,15 @@
         <v>2000</v>
       </c>
       <c r="K6" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>4</v>
@@ -1211,15 +1212,15 @@
         <v>0</v>
       </c>
       <c r="K7" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>4</v>
@@ -1246,7 +1247,7 @@
         <v>1500</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1278,10 +1279,10 @@
         <v>2017</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
@@ -1313,10 +1314,10 @@
         <v>2019</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K10" s="32" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1351,7 +1352,7 @@
         <v>1700</v>
       </c>
       <c r="K11" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1362,7 +1363,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="12">
         <v>552000</v>
@@ -1386,7 +1387,7 @@
         <v>2728</v>
       </c>
       <c r="K12" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1421,7 +1422,7 @@
         <v>3680</v>
       </c>
       <c r="K13" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1456,7 +1457,7 @@
         <v>3360</v>
       </c>
       <c r="K14" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1464,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>4</v>
@@ -1491,18 +1492,18 @@
         <v>2100</v>
       </c>
       <c r="K15" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="12">
         <v>367000</v>
@@ -1526,18 +1527,18 @@
         <v>1050</v>
       </c>
       <c r="K16" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>21</v>
-      </c>
       <c r="C17" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="12">
         <v>476000</v>
@@ -1561,18 +1562,18 @@
         <v>5024</v>
       </c>
       <c r="K17" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>23</v>
-      </c>
       <c r="C18" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="12">
         <v>340000</v>
@@ -1596,18 +1597,18 @@
         <v>2800</v>
       </c>
       <c r="K18" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="12">
         <v>466000</v>
@@ -1631,18 +1632,18 @@
         <v>0</v>
       </c>
       <c r="K19" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>26</v>
-      </c>
       <c r="C20" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="12">
         <v>508000</v>
@@ -1666,18 +1667,18 @@
         <v>3275</v>
       </c>
       <c r="K20" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>28</v>
-      </c>
       <c r="C21" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="12">
         <v>555000</v>
@@ -1701,18 +1702,18 @@
         <v>612</v>
       </c>
       <c r="K21" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="12">
         <v>528000</v>
@@ -1736,18 +1737,18 @@
         <v>1197</v>
       </c>
       <c r="K22" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="12">
         <v>383000</v>
@@ -1771,18 +1772,18 @@
         <v>2000</v>
       </c>
       <c r="K23" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" s="12">
         <v>348000</v>
@@ -1806,18 +1807,18 @@
         <v>2025</v>
       </c>
       <c r="K24" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="12">
         <v>396000</v>
@@ -1841,18 +1842,18 @@
         <v>2000</v>
       </c>
       <c r="K25" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" s="12">
         <v>293000</v>
@@ -1875,19 +1876,19 @@
       <c r="J26" s="26">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
-        <v>124</v>
+      <c r="K26" s="33" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="12">
         <v>730000</v>
@@ -1916,13 +1917,13 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" s="26">
         <v>405000</v>
@@ -1945,19 +1946,19 @@
       <c r="J28" s="26">
         <v>1050</v>
       </c>
-      <c r="K28" t="s">
-        <v>127</v>
+      <c r="K28" s="33" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" s="26">
         <v>450000</v>
@@ -1980,8 +1981,8 @@
       <c r="J29" s="26">
         <v>1050</v>
       </c>
-      <c r="K29" s="32" t="s">
-        <v>128</v>
+      <c r="K29" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2080,58 +2081,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="N1" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -2145,49 +2146,49 @@
         <v>8</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="14">
         <v>130</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="14">
         <v>8</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S2" s="30">
         <v>4</v>
@@ -2204,49 +2205,49 @@
         <v>7</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="14">
         <v>100</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" s="14">
         <v>4</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S3" s="30">
         <v>5</v>
@@ -2263,49 +2264,49 @@
         <v>4</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="14">
         <v>45</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="14">
         <v>2</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S4" s="30">
         <v>5</v>
@@ -2313,7 +2314,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="21">
         <v>6600</v>
@@ -2322,49 +2323,49 @@
         <v>1</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="22">
         <v>10</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="22">
         <v>1</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N5" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S5" s="30">
         <v>3</v>
@@ -2372,58 +2373,58 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="22">
         <v>1</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="22">
         <v>0</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q6" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S6" s="30">
         <v>5</v>
@@ -2431,58 +2432,58 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="22">
         <v>0</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="22">
         <v>1</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P7" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S7" s="30">
         <v>1</v>
@@ -2490,58 +2491,58 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="14">
         <v>1</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" s="14">
         <v>1</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S8" s="30">
         <v>1</v>
@@ -2552,55 +2553,55 @@
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="14">
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="14">
         <v>25</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I9" s="14">
         <v>1</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S9" s="30">
         <v>3</v>
@@ -2617,49 +2618,49 @@
         <v>2</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I10" s="14">
         <v>3</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S10" s="30">
         <v>4</v>
@@ -2676,49 +2677,49 @@
         <v>1</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" s="14">
         <v>1</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S11" s="30">
         <v>3</v>
@@ -2735,49 +2736,49 @@
         <v>3</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I12" s="14">
         <v>2</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S12" s="30">
         <v>5</v>
@@ -2788,55 +2789,55 @@
         <v>13</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="14">
         <v>1</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I13" s="14">
         <v>1</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S13" s="30">
         <v>3</v>
@@ -2853,49 +2854,49 @@
         <v>1</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="14">
         <v>1</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q14" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R14" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S14" s="30">
         <v>3</v>
@@ -2912,49 +2913,49 @@
         <v>1</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="H15" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" s="14">
         <v>2</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P15" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q15" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R15" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S15" s="30">
         <v>2</v>
@@ -2962,7 +2963,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="13">
         <v>2000</v>
@@ -2971,49 +2972,49 @@
         <v>1</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I16" s="14">
         <v>1</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S16" s="30">
         <v>1</v>
@@ -3021,7 +3022,7 @@
     </row>
     <row r="17" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="13">
         <v>1100</v>
@@ -3030,49 +3031,49 @@
         <v>5</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I17" s="14">
         <v>3</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P17" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q17" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R17" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S17" s="30">
         <v>4</v>
@@ -3080,7 +3081,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="13">
         <v>2600</v>
@@ -3089,49 +3090,49 @@
         <v>1</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="14">
         <v>50</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="14">
         <v>1</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S18" s="30">
         <v>3</v>
@@ -3139,7 +3140,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="13">
         <v>2500</v>
@@ -3148,49 +3149,49 @@
         <v>1</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I19" s="14">
         <v>1</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P19" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q19" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R19" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S19" s="30">
         <v>3</v>
@@ -3198,58 +3199,58 @@
     </row>
     <row r="20" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="14">
         <v>1</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I20" s="14">
         <v>1</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S20" s="30">
         <v>4</v>
@@ -3257,58 +3258,58 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="14">
         <v>0</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="14">
         <v>30</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="14">
         <v>1</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N21" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q21" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R21" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S21" s="30">
         <v>4</v>
@@ -3316,7 +3317,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="13">
         <v>2450</v>
@@ -3325,49 +3326,49 @@
         <v>1</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I22" s="14">
         <v>2</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q22" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S22" s="30">
         <v>3</v>
@@ -3375,7 +3376,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="13">
         <v>2000</v>
@@ -3384,49 +3385,49 @@
         <v>1</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I23" s="14">
         <v>1</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N23" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S23" s="30">
         <v>2</v>
@@ -3434,7 +3435,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="13">
         <v>2425</v>
@@ -3443,49 +3444,49 @@
         <v>1</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24" s="14">
         <v>1</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q24" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S24" s="30">
         <v>3</v>
@@ -3493,7 +3494,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="13">
         <v>2568</v>
@@ -3502,49 +3503,49 @@
         <v>2</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" s="14">
         <v>1</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q25" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S25" s="30">
         <v>3</v>
@@ -3552,58 +3553,58 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="14">
         <v>0</v>
       </c>
       <c r="D26" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="F26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I26" s="14">
         <v>1</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P26" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q26" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S26" s="30">
         <v>3</v>
@@ -3611,7 +3612,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="21">
         <v>5520</v>
@@ -3620,49 +3621,49 @@
         <v>1</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I27" s="22">
         <v>2</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K27" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O27" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q27" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S27" s="30">
         <v>4</v>
@@ -3670,7 +3671,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="21">
         <v>4500</v>
@@ -3679,49 +3680,49 @@
         <v>1</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="22">
         <v>25</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I28" s="22">
         <v>1</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K28" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L28" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O28" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P28" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q28" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R28" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S28" s="30">
         <v>5</v>
@@ -3729,58 +3730,58 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="22">
         <v>1</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I29" s="22">
         <v>1</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K29" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L29" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M29" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q29" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R29" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S29" s="30">
         <v>2</v>
@@ -3806,7 +3807,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>